<commit_message>
Graph ash small tree occurrence by species
</commit_message>
<xml_diff>
--- a/2011_data/2011 island lake_checked.xlsx
+++ b/2011_data/2011 island lake_checked.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/perry_1864_osu_edu/Documents/Documents/Perry Lab/Emerald Ash Borer Projects/2011 MI EAB Microplots_Wendy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/EAB_Michigan_2024_2025_github_folder/2011_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_8EE7DC17FAF763342ACB3AC849CCE6F08ECF2E1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3721D558-21D5-4701-BAF6-2F1F3264DEC2}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_8EE7DC17FAF763342ACB3AC849CCE6F08ECF2E1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50B56031-D5B5-443E-878B-77DF64DC241B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quads.all" sheetId="7" r:id="rId1"/>
@@ -952,7 +952,7 @@
     <numFmt numFmtId="164" formatCode="ddmmmyy"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1452,27 +1452,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="5" topLeftCell="H60" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="AA90" sqref="AA90"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="3" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="31" width="9.140625" style="1"/>
-    <col min="32" max="36" width="9.140625" style="9" customWidth="1"/>
-    <col min="38" max="38" width="29.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" hidden="1" customWidth="1"/>
+    <col min="8" max="31" width="9.1796875" style="1"/>
+    <col min="32" max="36" width="9.1796875" style="9" customWidth="1"/>
+    <col min="38" max="38" width="29.26953125" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1539,7 +1539,7 @@
       <c r="AJ1"/>
       <c r="AL1" s="28"/>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>3</v>
       </c>
@@ -1606,7 +1606,7 @@
       <c r="AJ2"/>
       <c r="AL2" s="28"/>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C3" s="16"/>
       <c r="N3"/>
       <c r="O3"/>
@@ -1627,7 +1627,7 @@
       <c r="AD3"/>
       <c r="AE3"/>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
@@ -1661,7 +1661,7 @@
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2011</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2011</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2011</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2011</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2011</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2011</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2011</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2011</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2011</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2011</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>84.5</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2011</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2011</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2011</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2011</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2011</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2011</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2011</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2011</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:38">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:38">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2011</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:38">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2011</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="36" spans="1:38">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2011</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:38">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2011</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:38">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2011</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:38">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2011</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="40" spans="1:38">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2011</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:38">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2011</v>
       </c>
@@ -5986,7 +5986,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:38">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2011</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:38">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:38">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2011</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:38">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2011</v>
       </c>
@@ -6460,7 +6460,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:38">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2011</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:38">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2011</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="48" spans="1:38">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2011</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="49" spans="1:38">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2011</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:38">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2011</v>
       </c>
@@ -7048,7 +7048,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:38">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2011</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2011</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:38">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2011</v>
       </c>
@@ -7399,7 +7399,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:38">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2011</v>
       </c>
@@ -7519,7 +7519,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:38">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2011</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:38">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2011</v>
       </c>
@@ -7756,7 +7756,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:38">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2011</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:38">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2011</v>
       </c>
@@ -7990,7 +7990,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:38">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2011</v>
       </c>
@@ -8107,7 +8107,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="60" spans="1:38">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2011</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="61" spans="1:38" s="32" customFormat="1">
+    <row r="61" spans="1:38" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="32">
         <v>2011</v>
       </c>
@@ -8342,7 +8342,7 @@
       </c>
       <c r="AL61" s="40"/>
     </row>
-    <row r="62" spans="1:38">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2011</v>
       </c>
@@ -8459,7 +8459,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="63" spans="1:38">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2011</v>
       </c>
@@ -8576,7 +8576,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="64" spans="1:38">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2011</v>
       </c>
@@ -8693,7 +8693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:38" s="32" customFormat="1">
+    <row r="65" spans="1:38" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="32">
         <v>2011</v>
       </c>
@@ -8811,7 +8811,7 @@
       </c>
       <c r="AL65" s="40"/>
     </row>
-    <row r="66" spans="1:38">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2011</v>
       </c>
@@ -8928,7 +8928,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="67" spans="1:38">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2011</v>
       </c>
@@ -9045,7 +9045,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="68" spans="1:38">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2011</v>
       </c>
@@ -9162,7 +9162,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="69" spans="1:38">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2011</v>
       </c>
@@ -9279,7 +9279,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="70" spans="1:38">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2011</v>
       </c>
@@ -9396,7 +9396,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="71" spans="1:38">
+    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2011</v>
       </c>
@@ -9513,7 +9513,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="72" spans="1:38" s="32" customFormat="1">
+    <row r="72" spans="1:38" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="32">
         <v>2011</v>
       </c>
@@ -9631,7 +9631,7 @@
       </c>
       <c r="AL72" s="40"/>
     </row>
-    <row r="73" spans="1:38">
+    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2011</v>
       </c>
@@ -9751,7 +9751,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:38">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2011</v>
       </c>
@@ -9871,7 +9871,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:38">
+    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2011</v>
       </c>
@@ -9988,7 +9988,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="76" spans="1:38">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2011</v>
       </c>
@@ -10105,7 +10105,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="77" spans="1:38">
+    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2011</v>
       </c>
@@ -10222,7 +10222,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="1:38">
+    <row r="78" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2011</v>
       </c>
@@ -10342,7 +10342,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:38">
+    <row r="79" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2011</v>
       </c>
@@ -10459,7 +10459,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="80" spans="1:38" s="32" customFormat="1">
+    <row r="80" spans="1:38" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="32">
         <v>2011</v>
       </c>
@@ -10579,7 +10579,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:38">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2011</v>
       </c>
@@ -10696,7 +10696,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="82" spans="1:38">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2011</v>
       </c>
@@ -10813,7 +10813,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="83" spans="1:38">
+    <row r="83" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2011</v>
       </c>
@@ -10933,7 +10933,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="1:38">
+    <row r="84" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2011</v>
       </c>
@@ -11050,7 +11050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:38">
+    <row r="85" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2011</v>
       </c>
@@ -11167,7 +11167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:38">
+    <row r="86" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2011</v>
       </c>
@@ -11284,7 +11284,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="87" spans="1:38">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2011</v>
       </c>
@@ -11401,7 +11401,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:38">
+    <row r="88" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B88" s="20"/>
       <c r="E88" s="20"/>
       <c r="H88" s="26"/>
@@ -11416,7 +11416,7 @@
       <c r="AJ88" s="22"/>
       <c r="AK88" s="22"/>
     </row>
-    <row r="89" spans="1:38">
+    <row r="89" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B89" s="20"/>
       <c r="E89" s="20"/>
       <c r="H89" s="26"/>
@@ -11431,26 +11431,26 @@
       <c r="AJ89" s="22"/>
       <c r="AK89" s="22"/>
     </row>
-    <row r="90" spans="1:38">
+    <row r="90" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B90" s="20"/>
       <c r="E90" s="20"/>
       <c r="AF90" s="22"/>
       <c r="AJ90" s="22"/>
       <c r="AK90" s="22"/>
     </row>
-    <row r="91" spans="1:38">
+    <row r="91" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B91" s="20"/>
     </row>
-    <row r="92" spans="1:38">
+    <row r="92" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B92" s="20"/>
     </row>
-    <row r="93" spans="1:38">
+    <row r="93" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B93" s="20"/>
     </row>
-    <row r="94" spans="1:38">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B94" s="20"/>
     </row>
-    <row r="95" spans="1:38">
+    <row r="95" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B95" s="20"/>
     </row>
   </sheetData>
@@ -11470,19 +11470,19 @@
       <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="28"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="8.81640625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
@@ -11511,7 +11511,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2011</v>
       </c>
@@ -11538,7 +11538,7 @@
       </c>
       <c r="J4" s="19"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -11564,7 +11564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2011</v>
       </c>
@@ -11590,7 +11590,7 @@
         <v>7125</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -11616,7 +11616,7 @@
         <v>7126</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2011</v>
       </c>
@@ -11642,7 +11642,7 @@
         <v>7127</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -11668,7 +11668,7 @@
         <v>7128</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -11695,7 +11695,7 @@
       </c>
       <c r="J10" s="19"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -11721,7 +11721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2011</v>
       </c>
@@ -11747,7 +11747,7 @@
         <v>8063</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -11773,7 +11773,7 @@
         <v>8064</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -11802,7 +11802,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -11828,7 +11828,7 @@
         <v>8071</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2011</v>
       </c>
@@ -11855,7 +11855,7 @@
       </c>
       <c r="J16" s="19"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2011</v>
       </c>
@@ -11881,7 +11881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2011</v>
       </c>
@@ -11907,7 +11907,7 @@
         <v>8050</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2011</v>
       </c>
@@ -11933,7 +11933,7 @@
         <v>8051</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2011</v>
       </c>
@@ -11959,7 +11959,7 @@
         <v>8052</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2011</v>
       </c>
@@ -11985,7 +11985,7 @@
         <v>8053</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2011</v>
       </c>
@@ -12015,7 +12015,7 @@
       </c>
       <c r="J22" s="19"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -12041,7 +12041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -12067,7 +12067,7 @@
         <v>7148</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2011</v>
       </c>
@@ -12093,7 +12093,7 @@
         <v>7149</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2011</v>
       </c>
@@ -12119,7 +12119,7 @@
         <v>7150</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2011</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2011</v>
       </c>
@@ -12172,7 +12172,7 @@
       </c>
       <c r="J28" s="19"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2011</v>
       </c>
@@ -12198,7 +12198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2011</v>
       </c>
@@ -12224,7 +12224,7 @@
         <v>8168</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2011</v>
       </c>
@@ -12250,7 +12250,7 @@
         <v>8169</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2011</v>
       </c>
@@ -12276,7 +12276,7 @@
         <v>8170</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -12302,7 +12302,7 @@
         <v>8171</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2011</v>
       </c>
@@ -12329,7 +12329,7 @@
       </c>
       <c r="J34" s="19"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2011</v>
       </c>
@@ -12355,7 +12355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2011</v>
       </c>
@@ -12381,7 +12381,7 @@
         <v>7514</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2011</v>
       </c>
@@ -12407,7 +12407,7 @@
         <v>7515</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2011</v>
       </c>
@@ -12433,7 +12433,7 @@
         <v>7516</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2011</v>
       </c>
@@ -12459,7 +12459,7 @@
         <v>7517</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2011</v>
       </c>
@@ -12486,7 +12486,7 @@
       </c>
       <c r="J40" s="19"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2011</v>
       </c>
@@ -12512,7 +12512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2011</v>
       </c>
@@ -12538,7 +12538,7 @@
         <v>8104</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -12564,7 +12564,7 @@
         <v>8105</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2011</v>
       </c>
@@ -12593,7 +12593,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2011</v>
       </c>
@@ -12619,7 +12619,7 @@
         <v>8107</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2011</v>
       </c>
@@ -12646,7 +12646,7 @@
       </c>
       <c r="J46" s="19"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2011</v>
       </c>
@@ -12675,7 +12675,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2011</v>
       </c>
@@ -12704,7 +12704,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2011</v>
       </c>
@@ -12730,7 +12730,7 @@
         <v>8094</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2011</v>
       </c>
@@ -12756,7 +12756,7 @@
         <v>8095</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2011</v>
       </c>
@@ -12782,7 +12782,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2011</v>
       </c>
@@ -12809,7 +12809,7 @@
       </c>
       <c r="J52" s="19"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2011</v>
       </c>
@@ -12838,7 +12838,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2011</v>
       </c>
@@ -12864,7 +12864,7 @@
         <v>8126</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2011</v>
       </c>
@@ -12890,7 +12890,7 @@
         <v>8127</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2011</v>
       </c>
@@ -12919,7 +12919,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2011</v>
       </c>
@@ -12948,7 +12948,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2011</v>
       </c>
@@ -12975,7 +12975,7 @@
       </c>
       <c r="J58" s="19"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2011</v>
       </c>
@@ -13001,7 +13001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2011</v>
       </c>
@@ -13030,7 +13030,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2011</v>
       </c>
@@ -13059,7 +13059,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2011</v>
       </c>
@@ -13088,7 +13088,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2011</v>
       </c>
@@ -13117,7 +13117,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2011</v>
       </c>
@@ -13144,7 +13144,7 @@
       </c>
       <c r="J64" s="19"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2011</v>
       </c>
@@ -13170,7 +13170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2011</v>
       </c>
@@ -13196,7 +13196,7 @@
         <v>7545</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2011</v>
       </c>
@@ -13222,7 +13222,7 @@
         <v>7546</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2011</v>
       </c>
@@ -13248,7 +13248,7 @@
         <v>7547</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2011</v>
       </c>
@@ -13274,7 +13274,7 @@
         <v>7548</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2011</v>
       </c>
@@ -13301,7 +13301,7 @@
       </c>
       <c r="J70" s="19"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2011</v>
       </c>
@@ -13327,7 +13327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2011</v>
       </c>
@@ -13356,7 +13356,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2011</v>
       </c>
@@ -13382,7 +13382,7 @@
         <v>7534</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2011</v>
       </c>
@@ -13408,7 +13408,7 @@
         <v>7535</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2011</v>
       </c>
@@ -13434,183 +13434,183 @@
         <v>7536</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B76" s="20"/>
       <c r="F76" s="20"/>
       <c r="H76" s="20"/>
       <c r="J76" s="19"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B77" s="20"/>
       <c r="G77" s="20"/>
       <c r="H77" s="20"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B78" s="20"/>
       <c r="H78" s="20"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B79" s="20"/>
       <c r="H79" s="20"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B80" s="20"/>
       <c r="F80" s="20"/>
       <c r="G80" s="20"/>
       <c r="H80" s="20"/>
     </row>
-    <row r="81" spans="2:10">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" s="20"/>
       <c r="G81" s="20"/>
       <c r="H81" s="20"/>
     </row>
-    <row r="82" spans="2:10">
+    <row r="82" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B82" s="20"/>
       <c r="F82" s="20"/>
       <c r="G82" s="20"/>
       <c r="H82" s="20"/>
       <c r="J82" s="19"/>
     </row>
-    <row r="83" spans="2:10">
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83" s="20"/>
       <c r="G83" s="20"/>
       <c r="H83" s="20"/>
     </row>
-    <row r="84" spans="2:10">
+    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B84" s="20"/>
       <c r="F84" s="20"/>
       <c r="G84" s="20"/>
       <c r="H84" s="20"/>
     </row>
-    <row r="85" spans="2:10">
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B85" s="20"/>
       <c r="G85" s="20"/>
       <c r="H85" s="20"/>
     </row>
-    <row r="86" spans="2:10">
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B86" s="20"/>
       <c r="F86" s="20"/>
       <c r="G86" s="20"/>
       <c r="H86" s="20"/>
     </row>
-    <row r="87" spans="2:10">
+    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B87" s="20"/>
       <c r="G87" s="20"/>
       <c r="H87" s="20"/>
     </row>
-    <row r="88" spans="2:10">
+    <row r="88" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B88" s="20"/>
       <c r="G88" s="20"/>
       <c r="H88" s="20"/>
       <c r="J88" s="19"/>
     </row>
-    <row r="89" spans="2:10">
+    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B89" s="20"/>
       <c r="G89" s="20"/>
       <c r="H89" s="20"/>
     </row>
-    <row r="90" spans="2:10">
+    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B90" s="20"/>
       <c r="G90" s="20"/>
       <c r="H90" s="20"/>
     </row>
-    <row r="91" spans="2:10">
+    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B91" s="20"/>
       <c r="G91" s="20"/>
       <c r="H91" s="20"/>
     </row>
-    <row r="92" spans="2:10">
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B92" s="20"/>
       <c r="G92" s="20"/>
       <c r="H92" s="20"/>
     </row>
-    <row r="93" spans="2:10">
+    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B93" s="20"/>
       <c r="G93" s="20"/>
       <c r="H93" s="20"/>
     </row>
-    <row r="94" spans="2:10">
+    <row r="94" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B94" s="20"/>
       <c r="G94" s="20"/>
       <c r="H94" s="20"/>
       <c r="J94" s="19"/>
     </row>
-    <row r="95" spans="2:10">
+    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B95" s="20"/>
       <c r="G95" s="20"/>
       <c r="H95" s="20"/>
     </row>
-    <row r="96" spans="2:10">
+    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B96" s="20"/>
       <c r="H96" s="20"/>
     </row>
-    <row r="97" spans="2:10">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B97" s="20"/>
       <c r="H97" s="20"/>
     </row>
-    <row r="98" spans="2:10">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B98" s="20"/>
       <c r="H98" s="20"/>
     </row>
-    <row r="99" spans="2:10">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B99" s="20"/>
       <c r="H99" s="20"/>
     </row>
-    <row r="100" spans="2:10">
+    <row r="100" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B100" s="20"/>
       <c r="F100" s="20"/>
       <c r="G100" s="20"/>
       <c r="H100" s="20"/>
       <c r="J100" s="19"/>
     </row>
-    <row r="101" spans="2:10">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B101" s="20"/>
       <c r="G101" s="20"/>
       <c r="H101" s="20"/>
     </row>
-    <row r="102" spans="2:10">
+    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B102" s="20"/>
       <c r="G102" s="20"/>
       <c r="H102" s="20"/>
     </row>
-    <row r="103" spans="2:10">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B103" s="20"/>
       <c r="G103" s="20"/>
     </row>
-    <row r="104" spans="2:10">
+    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B104" s="20"/>
       <c r="G104" s="20"/>
     </row>
-    <row r="105" spans="2:10">
+    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B105" s="20"/>
       <c r="G105" s="20"/>
     </row>
-    <row r="106" spans="2:10">
+    <row r="106" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B106" s="20"/>
       <c r="G106" s="20"/>
       <c r="H106" s="20"/>
       <c r="J106" s="19"/>
     </row>
-    <row r="107" spans="2:10">
+    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B107" s="20"/>
       <c r="G107" s="20"/>
       <c r="H107" s="20"/>
     </row>
-    <row r="108" spans="2:10">
+    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B108" s="20"/>
       <c r="G108" s="20"/>
       <c r="H108" s="20"/>
     </row>
-    <row r="109" spans="2:10">
+    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B109" s="20"/>
       <c r="G109" s="20"/>
       <c r="H109" s="20"/>
     </row>
-    <row r="110" spans="2:10">
+    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B110" s="20"/>
       <c r="H110" s="20"/>
     </row>
-    <row r="111" spans="2:10">
+    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B111" s="20"/>
       <c r="H111" s="20"/>
     </row>
@@ -13635,14 +13635,14 @@
       <selection pane="bottomLeft" activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>127</v>
       </c>
@@ -13656,7 +13656,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>128</v>
       </c>
@@ -13670,7 +13670,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -13681,7 +13681,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="13.5" thickBot="1">
+    <row r="4" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>8</v>
       </c>
@@ -13722,7 +13722,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="13.5" thickTop="1">
+    <row r="5" spans="1:13" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -13763,7 +13763,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2011</v>
       </c>
@@ -13804,7 +13804,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -13845,7 +13845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2011</v>
       </c>
@@ -13886,7 +13886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -13927,7 +13927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -13968,7 +13968,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -14009,7 +14009,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2011</v>
       </c>
@@ -14050,7 +14050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -14091,7 +14091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -14132,7 +14132,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -14173,7 +14173,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2011</v>
       </c>
@@ -14214,7 +14214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2011</v>
       </c>
@@ -14255,7 +14255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2011</v>
       </c>
@@ -14296,7 +14296,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2011</v>
       </c>
@@ -14337,7 +14337,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2011</v>
       </c>
@@ -14378,7 +14378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2011</v>
       </c>
@@ -14419,7 +14419,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2011</v>
       </c>
@@ -14460,7 +14460,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -14501,7 +14501,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -14542,7 +14542,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2011</v>
       </c>
@@ -14583,7 +14583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2011</v>
       </c>
@@ -14624,7 +14624,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2011</v>
       </c>
@@ -14665,7 +14665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2011</v>
       </c>
@@ -14706,7 +14706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2011</v>
       </c>
@@ -14747,7 +14747,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2011</v>
       </c>
@@ -14788,7 +14788,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2011</v>
       </c>
@@ -14829,7 +14829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2011</v>
       </c>
@@ -14870,7 +14870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -14911,7 +14911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2011</v>
       </c>
@@ -14952,7 +14952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2011</v>
       </c>
@@ -14993,7 +14993,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2011</v>
       </c>
@@ -15034,7 +15034,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2011</v>
       </c>
@@ -15075,7 +15075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2011</v>
       </c>
@@ -15116,7 +15116,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2011</v>
       </c>
@@ -15157,7 +15157,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2011</v>
       </c>
@@ -15198,7 +15198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2011</v>
       </c>
@@ -15239,7 +15239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2011</v>
       </c>
@@ -15280,7 +15280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -15321,7 +15321,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2011</v>
       </c>
@@ -15362,7 +15362,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2011</v>
       </c>
@@ -15403,7 +15403,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2011</v>
       </c>
@@ -15444,7 +15444,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2011</v>
       </c>
@@ -15485,7 +15485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E48" s="20"/>
       <c r="F48" s="20"/>
       <c r="G48" s="20"/>
@@ -15496,7 +15496,7 @@
       <c r="L48" s="20"/>
       <c r="M48" s="20"/>
     </row>
-    <row r="49" spans="5:13">
+    <row r="49" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
@@ -15507,7 +15507,7 @@
       <c r="L49" s="20"/>
       <c r="M49" s="20"/>
     </row>
-    <row r="50" spans="5:13">
+    <row r="50" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
       <c r="G50" s="20"/>
@@ -15518,7 +15518,7 @@
       <c r="L50" s="20"/>
       <c r="M50" s="20"/>
     </row>
-    <row r="51" spans="5:13">
+    <row r="51" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
@@ -15529,7 +15529,7 @@
       <c r="L51" s="20"/>
       <c r="M51" s="20"/>
     </row>
-    <row r="52" spans="5:13">
+    <row r="52" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E52" s="20"/>
       <c r="F52" s="20"/>
       <c r="G52" s="20"/>
@@ -15540,7 +15540,7 @@
       <c r="L52" s="20"/>
       <c r="M52" s="20"/>
     </row>
-    <row r="53" spans="5:13">
+    <row r="53" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E53" s="20"/>
       <c r="F53" s="20"/>
       <c r="G53" s="20"/>
@@ -15551,7 +15551,7 @@
       <c r="L53" s="20"/>
       <c r="M53" s="20"/>
     </row>
-    <row r="54" spans="5:13">
+    <row r="54" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E54" s="20"/>
       <c r="F54" s="20"/>
       <c r="G54" s="20"/>
@@ -15562,7 +15562,7 @@
       <c r="L54" s="20"/>
       <c r="M54" s="20"/>
     </row>
-    <row r="55" spans="5:13">
+    <row r="55" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
       <c r="G55" s="20"/>
@@ -15573,7 +15573,7 @@
       <c r="L55" s="20"/>
       <c r="M55" s="20"/>
     </row>
-    <row r="56" spans="5:13">
+    <row r="56" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E56" s="20"/>
       <c r="F56" s="20"/>
       <c r="G56" s="20"/>
@@ -15584,7 +15584,7 @@
       <c r="L56" s="20"/>
       <c r="M56" s="20"/>
     </row>
-    <row r="57" spans="5:13">
+    <row r="57" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E57" s="20"/>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
@@ -15595,7 +15595,7 @@
       <c r="L57" s="20"/>
       <c r="M57" s="20"/>
     </row>
-    <row r="58" spans="5:13">
+    <row r="58" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E58" s="20"/>
       <c r="F58" s="20"/>
       <c r="G58" s="20"/>
@@ -15606,7 +15606,7 @@
       <c r="L58" s="20"/>
       <c r="M58" s="20"/>
     </row>
-    <row r="59" spans="5:13">
+    <row r="59" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E59" s="20"/>
       <c r="F59" s="20"/>
       <c r="G59" s="20"/>
@@ -15617,7 +15617,7 @@
       <c r="L59" s="20"/>
       <c r="M59" s="20"/>
     </row>
-    <row r="60" spans="5:13">
+    <row r="60" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E60" s="20"/>
       <c r="F60" s="20"/>
       <c r="G60" s="20"/>
@@ -15628,7 +15628,7 @@
       <c r="L60" s="20"/>
       <c r="M60" s="20"/>
     </row>
-    <row r="61" spans="5:13">
+    <row r="61" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E61" s="20"/>
       <c r="F61" s="20"/>
       <c r="G61" s="20"/>
@@ -15639,7 +15639,7 @@
       <c r="L61" s="20"/>
       <c r="M61" s="20"/>
     </row>
-    <row r="62" spans="5:13">
+    <row r="62" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E62" s="20"/>
       <c r="F62" s="20"/>
       <c r="G62" s="20"/>
@@ -15650,7 +15650,7 @@
       <c r="L62" s="20"/>
       <c r="M62" s="20"/>
     </row>
-    <row r="63" spans="5:13">
+    <row r="63" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="20"/>
@@ -15661,7 +15661,7 @@
       <c r="L63" s="20"/>
       <c r="M63" s="20"/>
     </row>
-    <row r="64" spans="5:13">
+    <row r="64" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E64" s="20"/>
       <c r="F64" s="20"/>
       <c r="G64" s="20"/>
@@ -15672,7 +15672,7 @@
       <c r="L64" s="20"/>
       <c r="M64" s="20"/>
     </row>
-    <row r="65" spans="5:13">
+    <row r="65" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
       <c r="G65" s="20"/>
@@ -15683,7 +15683,7 @@
       <c r="L65" s="20"/>
       <c r="M65" s="20"/>
     </row>
-    <row r="66" spans="5:13">
+    <row r="66" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="20"/>
@@ -15694,7 +15694,7 @@
       <c r="L66" s="20"/>
       <c r="M66" s="20"/>
     </row>
-    <row r="67" spans="5:13">
+    <row r="67" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E67" s="20"/>
       <c r="F67" s="20"/>
       <c r="G67" s="20"/>
@@ -15705,7 +15705,7 @@
       <c r="L67" s="20"/>
       <c r="M67" s="20"/>
     </row>
-    <row r="68" spans="5:13">
+    <row r="68" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E68" s="20"/>
       <c r="F68" s="20"/>
       <c r="G68" s="20"/>
@@ -15716,7 +15716,7 @@
       <c r="L68" s="20"/>
       <c r="M68" s="20"/>
     </row>
-    <row r="69" spans="5:13">
+    <row r="69" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E69" s="20"/>
       <c r="F69" s="20"/>
       <c r="G69" s="20"/>
@@ -15727,7 +15727,7 @@
       <c r="L69" s="20"/>
       <c r="M69" s="20"/>
     </row>
-    <row r="70" spans="5:13">
+    <row r="70" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E70" s="20"/>
       <c r="F70" s="20"/>
       <c r="G70" s="20"/>
@@ -15738,7 +15738,7 @@
       <c r="L70" s="20"/>
       <c r="M70" s="20"/>
     </row>
-    <row r="71" spans="5:13">
+    <row r="71" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E71" s="20"/>
       <c r="F71" s="20"/>
       <c r="G71" s="20"/>
@@ -15749,7 +15749,7 @@
       <c r="L71" s="20"/>
       <c r="M71" s="20"/>
     </row>
-    <row r="72" spans="5:13">
+    <row r="72" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E72" s="20"/>
       <c r="F72" s="20"/>
       <c r="G72" s="20"/>
@@ -15760,7 +15760,7 @@
       <c r="L72" s="20"/>
       <c r="M72" s="20"/>
     </row>
-    <row r="73" spans="5:13">
+    <row r="73" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E73" s="20"/>
       <c r="F73" s="20"/>
       <c r="G73" s="20"/>
@@ -15771,7 +15771,7 @@
       <c r="L73" s="20"/>
       <c r="M73" s="20"/>
     </row>
-    <row r="74" spans="5:13">
+    <row r="74" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E74" s="20"/>
       <c r="F74" s="20"/>
       <c r="G74" s="20"/>
@@ -15782,7 +15782,7 @@
       <c r="L74" s="20"/>
       <c r="M74" s="20"/>
     </row>
-    <row r="75" spans="5:13">
+    <row r="75" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E75" s="20"/>
       <c r="F75" s="20"/>
       <c r="G75" s="20"/>
@@ -15793,7 +15793,7 @@
       <c r="L75" s="20"/>
       <c r="M75" s="20"/>
     </row>
-    <row r="76" spans="5:13">
+    <row r="76" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E76" s="20"/>
       <c r="F76" s="20"/>
       <c r="G76" s="20"/>
@@ -15804,7 +15804,7 @@
       <c r="L76" s="20"/>
       <c r="M76" s="20"/>
     </row>
-    <row r="77" spans="5:13">
+    <row r="77" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E77" s="20"/>
       <c r="F77" s="20"/>
       <c r="G77" s="20"/>
@@ -15815,7 +15815,7 @@
       <c r="L77" s="20"/>
       <c r="M77" s="20"/>
     </row>
-    <row r="78" spans="5:13">
+    <row r="78" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E78" s="20"/>
       <c r="F78" s="20"/>
       <c r="G78" s="20"/>
@@ -15826,7 +15826,7 @@
       <c r="L78" s="20"/>
       <c r="M78" s="20"/>
     </row>
-    <row r="79" spans="5:13">
+    <row r="79" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E79" s="20"/>
       <c r="F79" s="20"/>
       <c r="G79" s="20"/>
@@ -15847,20 +15847,20 @@
   <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I106" sqref="I106"/>
+      <pane ySplit="3" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="28"/>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.26953125" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -15872,12 +15872,12 @@
         <v>201.06175999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.5" thickBot="1">
+    <row r="3" spans="1:11" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>8</v>
       </c>
@@ -15912,7 +15912,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.5" thickTop="1">
+    <row r="4" spans="1:11" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2011</v>
       </c>
@@ -15945,7 +15945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -15981,7 +15981,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2011</v>
       </c>
@@ -16014,7 +16014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -16047,7 +16047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2011</v>
       </c>
@@ -16080,7 +16080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -16117,7 +16117,7 @@
         <v>11.370000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -16153,7 +16153,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -16186,7 +16186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2011</v>
       </c>
@@ -16219,7 +16219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -16255,7 +16255,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -16288,7 +16288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -16324,7 +16324,7 @@
         <v>14.070000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2011</v>
       </c>
@@ -16361,7 +16361,7 @@
         <v>38.190000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2011</v>
       </c>
@@ -16397,7 +16397,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2011</v>
       </c>
@@ -16433,7 +16433,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2011</v>
       </c>
@@ -16469,7 +16469,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2011</v>
       </c>
@@ -16502,7 +16502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2011</v>
       </c>
@@ -16532,7 +16532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2011</v>
       </c>
@@ -16569,7 +16569,7 @@
         <v>80.400000000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -16603,7 +16603,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -16636,7 +16636,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2011</v>
       </c>
@@ -16669,7 +16669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2011</v>
       </c>
@@ -16702,7 +16702,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2011</v>
       </c>
@@ -16735,7 +16735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2011</v>
       </c>
@@ -16768,7 +16768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2011</v>
       </c>
@@ -16801,7 +16801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2011</v>
       </c>
@@ -16834,7 +16834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2011</v>
       </c>
@@ -16867,7 +16867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2011</v>
       </c>
@@ -16904,7 +16904,7 @@
         <v>42.21</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -16940,7 +16940,7 @@
         <v>18.09</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2011</v>
       </c>
@@ -16974,7 +16974,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2011</v>
       </c>
@@ -17009,7 +17009,7 @@
         <v>4.0200000000000005</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2011</v>
       </c>
@@ -17042,7 +17042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2011</v>
       </c>
@@ -17078,7 +17078,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2011</v>
       </c>
@@ -17114,7 +17114,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2011</v>
       </c>
@@ -17147,7 +17147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2011</v>
       </c>
@@ -17184,7 +17184,7 @@
         <v>60.570000000000007</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2011</v>
       </c>
@@ -17220,7 +17220,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2011</v>
       </c>
@@ -17253,7 +17253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -17286,7 +17286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2011</v>
       </c>
@@ -17322,7 +17322,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2011</v>
       </c>
@@ -17355,7 +17355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2011</v>
       </c>
@@ -17388,7 +17388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2011</v>
       </c>
@@ -17423,7 +17423,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2011</v>
       </c>
@@ -17457,7 +17457,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2011</v>
       </c>
@@ -17493,7 +17493,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2011</v>
       </c>
@@ -17526,7 +17526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2011</v>
       </c>
@@ -17562,7 +17562,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2011</v>
       </c>
@@ -17595,7 +17595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2011</v>
       </c>
@@ -17630,7 +17630,7 @@
         <v>26.130000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2011</v>
       </c>
@@ -17667,7 +17667,7 @@
         <v>44.400000000000006</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2011</v>
       </c>
@@ -17702,7 +17702,7 @@
         <v>4.0200000000000005</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2011</v>
       </c>
@@ -17739,7 +17739,7 @@
         <v>17.060000000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2011</v>
       </c>
@@ -17776,7 +17776,7 @@
         <v>16.439999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2011</v>
       </c>
@@ -17811,7 +17811,7 @@
         <v>6.0300000000000011</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2011</v>
       </c>
@@ -17847,7 +17847,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2011</v>
       </c>
@@ -17880,7 +17880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2011</v>
       </c>
@@ -17913,7 +17913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2011</v>
       </c>
@@ -17948,7 +17948,7 @@
         <v>12.739999999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2011</v>
       </c>
@@ -17979,7 +17979,7 @@
         <v>4.0200000000000005</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2011</v>
       </c>
@@ -18015,7 +18015,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2011</v>
       </c>
@@ -18049,7 +18049,7 @@
         <v>4.0200000000000005</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2011</v>
       </c>
@@ -18083,7 +18083,7 @@
         <v>4.0200000000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2011</v>
       </c>
@@ -18117,7 +18117,7 @@
         <v>4.0200000000000005</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2011</v>
       </c>
@@ -18153,7 +18153,7 @@
         <v>7.88</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2011</v>
       </c>
@@ -18188,7 +18188,7 @@
         <v>3.2100000000000004</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2011</v>
       </c>
@@ -18223,7 +18223,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2011</v>
       </c>
@@ -18257,7 +18257,7 @@
         <v>6.0299999999999994</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2011</v>
       </c>
@@ -18290,7 +18290,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2011</v>
       </c>
@@ -18326,7 +18326,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2011</v>
       </c>
@@ -18359,7 +18359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2011</v>
       </c>
@@ -18394,7 +18394,7 @@
         <v>6.0300000000000011</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2011</v>
       </c>
@@ -18429,7 +18429,7 @@
         <v>2.91</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2011</v>
       </c>
@@ -18466,7 +18466,7 @@
         <v>21.860000000000003</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2011</v>
       </c>
@@ -18500,7 +18500,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2011</v>
       </c>
@@ -18534,7 +18534,7 @@
         <v>2.0100000000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2011</v>
       </c>
@@ -18568,7 +18568,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2011</v>
       </c>
@@ -18601,7 +18601,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2011</v>
       </c>
@@ -18634,7 +18634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2011</v>
       </c>
@@ -18667,7 +18667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2011</v>
       </c>
@@ -18703,7 +18703,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2011</v>
       </c>
@@ -18739,7 +18739,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2011</v>
       </c>
@@ -18772,7 +18772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2011</v>
       </c>
@@ -18805,7 +18805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2011</v>
       </c>
@@ -18842,7 +18842,7 @@
         <v>52.500000000000007</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2011</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v>42.91</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2011</v>
       </c>
@@ -18912,7 +18912,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2011</v>
       </c>
@@ -18946,7 +18946,7 @@
         <v>2.0100000000000002</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2011</v>
       </c>
@@ -18982,7 +18982,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2011</v>
       </c>
@@ -19015,7 +19015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2011</v>
       </c>
@@ -19048,7 +19048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2011</v>
       </c>
@@ -19081,7 +19081,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2011</v>
       </c>
@@ -19114,7 +19114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2011</v>
       </c>
@@ -19151,7 +19151,7 @@
         <v>64.320000000000007</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2011</v>
       </c>
@@ -19187,7 +19187,7 @@
         <v>18.09</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2011</v>
       </c>
@@ -19221,7 +19221,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2011</v>
       </c>
@@ -19256,7 +19256,7 @@
         <v>1.3599999999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2011</v>
       </c>
@@ -19290,7 +19290,7 @@
         <v>2.2399999999999998</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2011</v>
       </c>
@@ -19326,7 +19326,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2011</v>
       </c>
@@ -19359,7 +19359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2011</v>
       </c>
@@ -19394,7 +19394,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2011</v>
       </c>
@@ -19428,7 +19428,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2011</v>
       </c>
@@ -19473,25 +19473,25 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="28"/>
+    <col min="10" max="10" width="8.81640625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.5" thickBot="1">
+    <row r="3" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>8</v>
       </c>
@@ -19523,7 +19523,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.5" thickTop="1">
+    <row r="4" spans="1:10" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2011</v>
       </c>
@@ -19552,7 +19552,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -19581,7 +19581,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2011</v>
       </c>
@@ -19610,7 +19610,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -19639,7 +19639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2011</v>
       </c>
@@ -19671,7 +19671,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -19703,7 +19703,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -19735,7 +19735,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -19767,7 +19767,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2011</v>
       </c>
@@ -19799,7 +19799,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -19831,7 +19831,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -19863,7 +19863,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -19895,7 +19895,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2011</v>
       </c>
@@ -19924,7 +19924,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2011</v>
       </c>
@@ -19956,7 +19956,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2011</v>
       </c>
@@ -19988,7 +19988,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2011</v>
       </c>
@@ -20017,7 +20017,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2011</v>
       </c>
@@ -20049,7 +20049,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2011</v>
       </c>
@@ -20078,7 +20078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2011</v>
       </c>
@@ -20107,7 +20107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -20136,7 +20136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -20165,7 +20165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2011</v>
       </c>
@@ -20197,7 +20197,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2011</v>
       </c>
@@ -20229,7 +20229,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2011</v>
       </c>
@@ -20261,7 +20261,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2011</v>
       </c>
@@ -20293,7 +20293,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2011</v>
       </c>
@@ -20325,7 +20325,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2011</v>
       </c>
@@ -20357,7 +20357,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2011</v>
       </c>
@@ -20389,7 +20389,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2011</v>
       </c>
@@ -20421,7 +20421,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -20453,7 +20453,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2011</v>
       </c>
@@ -20482,7 +20482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2011</v>
       </c>
@@ -20514,7 +20514,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2011</v>
       </c>
@@ -20543,7 +20543,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2011</v>
       </c>
@@ -20575,7 +20575,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2011</v>
       </c>
@@ -20604,7 +20604,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2011</v>
       </c>
@@ -20633,7 +20633,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2011</v>
       </c>
@@ -20665,7 +20665,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2011</v>
       </c>
@@ -20697,7 +20697,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2011</v>
       </c>
@@ -20729,7 +20729,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -20761,7 +20761,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2011</v>
       </c>
@@ -20793,7 +20793,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2011</v>
       </c>
@@ -20822,7 +20822,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2011</v>
       </c>
@@ -20854,7 +20854,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2011</v>
       </c>
@@ -20886,25 +20886,25 @@
         <v>185</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" s="20"/>
       <c r="G48" s="20"/>
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
     </row>
-    <row r="49" spans="2:9">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="20"/>
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
       <c r="I49" s="20"/>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="20"/>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="20"/>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="20"/>
     </row>
   </sheetData>
@@ -20919,29 +20919,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" ySplit="4" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="10" customWidth="1"/>
-    <col min="23" max="23" width="39.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7265625" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="4" customWidth="1"/>
+    <col min="9" max="10" width="9.1796875" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" style="10" customWidth="1"/>
+    <col min="13" max="13" width="21.54296875" customWidth="1"/>
+    <col min="14" max="14" width="11.81640625" customWidth="1"/>
+    <col min="20" max="20" width="9.1796875" style="10" customWidth="1"/>
+    <col min="23" max="23" width="39.7265625" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>192</v>
       </c>
@@ -20950,7 +20950,7 @@
       <c r="N1" s="9"/>
       <c r="W1" s="27"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>193</v>
       </c>
@@ -20959,7 +20959,7 @@
       <c r="N2" s="9"/>
       <c r="W2" s="27"/>
     </row>
-    <row r="3" spans="1:23" s="3" customFormat="1">
+    <row r="3" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="12"/>
       <c r="E3" s="9" t="s">
         <v>194</v>
@@ -20996,7 +20996,7 @@
       <c r="T3" s="17"/>
       <c r="W3" s="27"/>
     </row>
-    <row r="4" spans="1:23" s="7" customFormat="1" ht="13.5" thickBot="1">
+    <row r="4" spans="1:23" s="7" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
@@ -21067,7 +21067,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="13.5" thickTop="1">
+    <row r="5" spans="1:23" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -21129,7 +21129,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2011</v>
       </c>
@@ -21191,7 +21191,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -21256,7 +21256,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2011</v>
       </c>
@@ -21318,7 +21318,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -21380,7 +21380,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -21445,7 +21445,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -21510,7 +21510,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2011</v>
       </c>
@@ -21572,7 +21572,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -21637,7 +21637,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -21699,7 +21699,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -21764,7 +21764,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2011</v>
       </c>
@@ -21826,7 +21826,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2011</v>
       </c>
@@ -21888,7 +21888,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2011</v>
       </c>
@@ -21950,7 +21950,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2011</v>
       </c>
@@ -22012,7 +22012,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2011</v>
       </c>
@@ -22077,7 +22077,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2011</v>
       </c>
@@ -22142,7 +22142,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2011</v>
       </c>
@@ -22204,7 +22204,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -22269,7 +22269,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -22331,7 +22331,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2011</v>
       </c>
@@ -22396,7 +22396,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2011</v>
       </c>
@@ -22458,7 +22458,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2011</v>
       </c>
@@ -22523,7 +22523,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2011</v>
       </c>
@@ -22586,7 +22586,7 @@
       </c>
       <c r="W28" s="29"/>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2011</v>
       </c>
@@ -22651,7 +22651,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2011</v>
       </c>
@@ -22716,7 +22716,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2011</v>
       </c>
@@ -22778,7 +22778,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2011</v>
       </c>
@@ -22840,7 +22840,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -22905,7 +22905,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2011</v>
       </c>
@@ -22970,7 +22970,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2011</v>
       </c>
@@ -23035,7 +23035,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2011</v>
       </c>
@@ -23100,7 +23100,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2011</v>
       </c>
@@ -23165,7 +23165,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2011</v>
       </c>
@@ -23230,7 +23230,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2011</v>
       </c>
@@ -23295,7 +23295,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2011</v>
       </c>
@@ -23360,7 +23360,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2011</v>
       </c>
@@ -23425,7 +23425,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2011</v>
       </c>
@@ -23490,7 +23490,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -23555,7 +23555,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2011</v>
       </c>
@@ -23620,7 +23620,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="45" spans="1:23">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2011</v>
       </c>
@@ -23682,7 +23682,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="46" spans="1:23">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2011</v>
       </c>
@@ -23744,7 +23744,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B47" s="20"/>
       <c r="E47" s="22"/>
       <c r="F47" s="23"/>
@@ -23755,7 +23755,7 @@
       <c r="Q47" s="20"/>
       <c r="V47" s="20"/>
     </row>
-    <row r="48" spans="1:23">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B48" s="20"/>
       <c r="E48" s="22"/>
       <c r="F48" s="23"/>
@@ -23766,7 +23766,7 @@
       <c r="Q48" s="20"/>
       <c r="V48" s="20"/>
     </row>
-    <row r="49" spans="2:22">
+    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B49" s="20"/>
       <c r="E49" s="22"/>
       <c r="F49" s="23"/>
@@ -23777,7 +23777,7 @@
       <c r="Q49" s="20"/>
       <c r="V49" s="20"/>
     </row>
-    <row r="50" spans="2:22">
+    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B50" s="20"/>
       <c r="E50" s="22"/>
       <c r="F50" s="23"/>
@@ -23788,7 +23788,7 @@
       <c r="Q50" s="20"/>
       <c r="V50" s="20"/>
     </row>
-    <row r="51" spans="2:22">
+    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B51" s="20"/>
       <c r="E51" s="22"/>
       <c r="F51" s="23"/>
@@ -23799,7 +23799,7 @@
       <c r="Q51" s="20"/>
       <c r="V51" s="20"/>
     </row>
-    <row r="52" spans="2:22">
+    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B52" s="20"/>
       <c r="E52" s="22"/>
       <c r="F52" s="23"/>
@@ -23810,7 +23810,7 @@
       <c r="Q52" s="20"/>
       <c r="V52" s="20"/>
     </row>
-    <row r="53" spans="2:22">
+    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B53" s="20"/>
       <c r="E53" s="22"/>
       <c r="F53" s="23"/>
@@ -23821,7 +23821,7 @@
       <c r="Q53" s="20"/>
       <c r="V53" s="20"/>
     </row>
-    <row r="54" spans="2:22">
+    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B54" s="20"/>
       <c r="E54" s="22"/>
       <c r="F54" s="23"/>
@@ -23832,7 +23832,7 @@
       <c r="Q54" s="20"/>
       <c r="V54" s="20"/>
     </row>
-    <row r="55" spans="2:22">
+    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B55" s="20"/>
       <c r="E55" s="22"/>
       <c r="F55" s="23"/>
@@ -23843,7 +23843,7 @@
       <c r="Q55" s="20"/>
       <c r="V55" s="20"/>
     </row>
-    <row r="56" spans="2:22">
+    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B56" s="20"/>
       <c r="E56" s="22"/>
       <c r="F56" s="23"/>
@@ -23854,7 +23854,7 @@
       <c r="Q56" s="20"/>
       <c r="V56" s="20"/>
     </row>
-    <row r="57" spans="2:22">
+    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B57" s="20"/>
       <c r="E57" s="22"/>
       <c r="F57" s="23"/>
@@ -23865,7 +23865,7 @@
       <c r="Q57" s="20"/>
       <c r="V57" s="20"/>
     </row>
-    <row r="58" spans="2:22">
+    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B58" s="20"/>
       <c r="E58" s="22"/>
       <c r="F58" s="23"/>
@@ -23876,7 +23876,7 @@
       <c r="Q58" s="20"/>
       <c r="V58" s="20"/>
     </row>
-    <row r="59" spans="2:22">
+    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B59" s="20"/>
       <c r="E59" s="22"/>
       <c r="F59" s="23"/>
@@ -23890,7 +23890,7 @@
       <c r="Q59" s="20"/>
       <c r="V59" s="20"/>
     </row>
-    <row r="60" spans="2:22">
+    <row r="60" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B60" s="20"/>
       <c r="E60" s="22"/>
       <c r="F60" s="23"/>
@@ -23904,7 +23904,7 @@
       <c r="Q60" s="20"/>
       <c r="V60" s="20"/>
     </row>
-    <row r="61" spans="2:22">
+    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B61" s="20"/>
       <c r="E61" s="22"/>
       <c r="F61" s="23"/>
@@ -23918,7 +23918,7 @@
       <c r="Q61" s="20"/>
       <c r="V61" s="20"/>
     </row>
-    <row r="62" spans="2:22">
+    <row r="62" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B62" s="20"/>
       <c r="E62" s="22"/>
       <c r="F62" s="23"/>
@@ -23932,7 +23932,7 @@
       <c r="Q62" s="20"/>
       <c r="V62" s="20"/>
     </row>
-    <row r="63" spans="2:22">
+    <row r="63" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B63" s="20"/>
       <c r="E63" s="22"/>
       <c r="F63" s="23"/>
@@ -23942,7 +23942,7 @@
       <c r="P63" s="20"/>
       <c r="Q63" s="20"/>
     </row>
-    <row r="64" spans="2:22">
+    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B64" s="20"/>
       <c r="E64" s="22"/>
       <c r="F64" s="23"/>
@@ -23956,7 +23956,7 @@
       <c r="Q64" s="20"/>
       <c r="V64" s="20"/>
     </row>
-    <row r="65" spans="2:22">
+    <row r="65" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B65" s="20"/>
       <c r="E65" s="22"/>
       <c r="F65" s="23"/>
@@ -23966,7 +23966,7 @@
       <c r="P65" s="20"/>
       <c r="Q65" s="20"/>
     </row>
-    <row r="66" spans="2:22">
+    <row r="66" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B66" s="20"/>
       <c r="E66" s="22"/>
       <c r="F66" s="23"/>
@@ -23976,7 +23976,7 @@
       <c r="P66" s="20"/>
       <c r="Q66" s="20"/>
     </row>
-    <row r="67" spans="2:22">
+    <row r="67" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B67" s="20"/>
       <c r="E67" s="22"/>
       <c r="F67" s="23"/>
@@ -23986,7 +23986,7 @@
       <c r="P67" s="20"/>
       <c r="Q67" s="20"/>
     </row>
-    <row r="68" spans="2:22">
+    <row r="68" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B68" s="20"/>
       <c r="E68" s="22"/>
       <c r="F68" s="23"/>
@@ -23996,7 +23996,7 @@
       <c r="P68" s="20"/>
       <c r="Q68" s="20"/>
     </row>
-    <row r="69" spans="2:22">
+    <row r="69" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B69" s="20"/>
       <c r="E69" s="22"/>
       <c r="F69" s="23"/>
@@ -24006,7 +24006,7 @@
       <c r="P69" s="20"/>
       <c r="Q69" s="20"/>
     </row>
-    <row r="70" spans="2:22">
+    <row r="70" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B70" s="20"/>
       <c r="E70" s="22"/>
       <c r="F70" s="23"/>
@@ -24016,7 +24016,7 @@
       <c r="P70" s="20"/>
       <c r="Q70" s="20"/>
     </row>
-    <row r="71" spans="2:22">
+    <row r="71" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B71" s="20"/>
       <c r="E71" s="22"/>
       <c r="F71" s="23"/>
@@ -24026,7 +24026,7 @@
       <c r="P71" s="20"/>
       <c r="Q71" s="20"/>
     </row>
-    <row r="72" spans="2:22">
+    <row r="72" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B72" s="20"/>
       <c r="E72" s="22"/>
       <c r="F72" s="23"/>
@@ -24038,7 +24038,7 @@
       <c r="Q72" s="20"/>
       <c r="V72" s="20"/>
     </row>
-    <row r="73" spans="2:22">
+    <row r="73" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B73" s="20"/>
       <c r="E73" s="22"/>
       <c r="F73" s="23"/>
@@ -24050,7 +24050,7 @@
       <c r="Q73" s="20"/>
       <c r="V73" s="20"/>
     </row>
-    <row r="74" spans="2:22">
+    <row r="74" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B74" s="20"/>
       <c r="E74" s="22"/>
       <c r="F74" s="23"/>
@@ -24064,7 +24064,7 @@
       <c r="Q74" s="20"/>
       <c r="V74" s="20"/>
     </row>
-    <row r="75" spans="2:22">
+    <row r="75" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B75" s="20"/>
       <c r="E75" s="22"/>
       <c r="F75" s="23"/>
@@ -24078,7 +24078,7 @@
       <c r="Q75" s="20"/>
       <c r="V75" s="20"/>
     </row>
-    <row r="76" spans="2:22">
+    <row r="76" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B76" s="20"/>
       <c r="E76" s="22"/>
       <c r="F76" s="23"/>
@@ -24092,7 +24092,7 @@
       <c r="Q76" s="20"/>
       <c r="V76" s="20"/>
     </row>
-    <row r="77" spans="2:22">
+    <row r="77" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B77" s="20"/>
       <c r="E77" s="22"/>
       <c r="F77" s="23"/>
@@ -24106,7 +24106,7 @@
       <c r="Q77" s="20"/>
       <c r="V77" s="20"/>
     </row>
-    <row r="78" spans="2:22">
+    <row r="78" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B78" s="20"/>
       <c r="E78" s="22"/>
       <c r="F78" s="23"/>
@@ -24120,19 +24120,19 @@
       <c r="Q78" s="20"/>
       <c r="V78" s="20"/>
     </row>
-    <row r="79" spans="2:22">
+    <row r="79" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B79" s="20"/>
     </row>
-    <row r="80" spans="2:22">
+    <row r="80" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B80" s="20"/>
     </row>
-    <row r="81" spans="2:2">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="20"/>
     </row>
-    <row r="82" spans="2:2">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="20"/>
     </row>
-    <row r="83" spans="2:2">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="20"/>
     </row>
   </sheetData>
@@ -24160,15 +24160,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100838CD1DE87728B4A91AC01A490840121" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0286a0c1720992b0cd926edcb110b1cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6f6290a-188c-431b-bc1b-08909b9edd3c" xmlns:ns3="c4dec4b6-adc0-4ae7-a610-9837ec16b1be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fcb779e9d849f44277e6e1dd1ee1357" ns2:_="" ns3:_="">
     <xsd:import namespace="f6f6290a-188c-431b-bc1b-08909b9edd3c"/>
@@ -24381,14 +24372,49 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77456801-30CA-4A2B-8ECE-37929DAD51E2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77456801-30CA-4A2B-8ECE-37929DAD51E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c4dec4b6-adc0-4ae7-a610-9837ec16b1be"/>
+    <ds:schemaRef ds:uri="f6f6290a-188c-431b-bc1b-08909b9edd3c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63AA6421-B92B-46D9-A0AB-511FD1656E7F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76764107-DABE-49C4-8760-1862FA4F5426}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f6f6290a-188c-431b-bc1b-08909b9edd3c"/>
+    <ds:schemaRef ds:uri="c4dec4b6-adc0-4ae7-a610-9837ec16b1be"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76764107-DABE-49C4-8760-1862FA4F5426}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63AA6421-B92B-46D9-A0AB-511FD1656E7F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>